<commit_message>
2024/25 refreshment on the content
</commit_message>
<xml_diff>
--- a/MiniMiMo_HW_CPE_Model/MiniMiMo_Assembler.xlsx
+++ b/MiniMiMo_HW_CPE_Model/MiniMiMo_Assembler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unilj-my.sharepoint.com/personal/rozman_fri1_uni-lj_si/Documents/Delovni/Sluzba/MiMoEVO/MiniMiMo_Hardwired/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unilj-my.sharepoint.com/personal/rozman_fri1_uni-lj_si/Documents/Delovni/Sluzba/Predavanja/RA/Predavanja_24_25/Pogl_06_CPE/MiniMiMo_HW_CPE_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{F42BBA46-C848-4C20-8383-D5282208A516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48922C2D-CE88-4044-94CF-6F1B90F25C3D}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{F42BBA46-C848-4C20-8383-D5282208A516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1326FD1-86C7-4E2D-BDFF-F5A1F1FFB551}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{6CA5DDAA-0BF2-4A35-997C-05C062425F32}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{6CA5DDAA-0BF2-4A35-997C-05C062425F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Zbirnik" sheetId="1" r:id="rId1"/>
@@ -279,9 +279,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sistemov Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pisarna">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -319,7 +319,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pisarna">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -425,7 +425,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pisarna">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -567,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,22 +575,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA144E0-F21F-4D99-B819-0BCCE21AFC96}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="5" width="8.7265625" style="3"/>
     <col min="6" max="6" width="18" style="3" customWidth="1"/>
     <col min="7" max="8" width="8.7265625" style="3"/>
     <col min="9" max="9" width="13.81640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -651,12 +651,8 @@
         <f>DEC2HEX(F2*HEX2DEC("1000")+(G2*4+H2)*HEX2DEC("100")+E2)</f>
         <v>E020</v>
       </c>
-      <c r="N2">
-        <f>HEX2DEC("FF")*2</f>
-        <v>510</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -686,7 +682,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -719,7 +715,7 @@
         <v>E021</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -749,7 +745,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -779,7 +775,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -812,7 +808,7 @@
         <v>E022</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -842,7 +838,7 @@
         <v>5800</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -875,7 +871,7 @@
         <v>F007</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -896,7 +892,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -917,7 +913,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -938,7 +934,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -959,7 +955,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -980,7 +976,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1001,7 +997,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1412,13 +1408,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF1CB2F-70B3-485C-B1D8-73708F38D854}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" customWidth="1"/>
     <col min="3" max="5" width="8.7265625" style="3"/>
     <col min="6" max="6" width="18" style="3" customWidth="1"/>
     <col min="7" max="8" width="8.7265625" style="3"/>

</xml_diff>